<commit_message>
Almost finished Data Dictionnary
</commit_message>
<xml_diff>
--- a/Fonctionnelle/Dictionnaire_Donnees.xlsx
+++ b/Fonctionnelle/Dictionnaire_Donnees.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="PlayerCharacter" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,18 @@
     <sheet name="Item" sheetId="7" r:id="rId7"/>
     <sheet name="ItemCategory" sheetId="8" r:id="rId8"/>
     <sheet name="EncounterDrop" sheetId="9" r:id="rId9"/>
+    <sheet name="Encounter" sheetId="11" r:id="rId10"/>
+    <sheet name="Monster" sheetId="12" r:id="rId11"/>
+    <sheet name="Avatar" sheetId="13" r:id="rId12"/>
+    <sheet name="Structure" sheetId="14" r:id="rId13"/>
+    <sheet name="NonPlayerCharacter" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="287">
   <si>
     <t>Nom du champ</t>
   </si>
@@ -717,12 +722,6 @@
     <t>Indicateur des chances de laisser un objet</t>
   </si>
   <si>
-    <t>Quantité minimale de l'objet</t>
-  </si>
-  <si>
-    <t>Quantité maximale de l'objet</t>
-  </si>
-  <si>
     <t>EncounterDrop</t>
   </si>
   <si>
@@ -732,7 +731,163 @@
     <t>Entier Court Non-Signé</t>
   </si>
   <si>
-    <t>MinGold</t>
+    <t>Quantité minimale d'objets abandonnés</t>
+  </si>
+  <si>
+    <t>Quantité maximale d'objets abandonnés</t>
+  </si>
+  <si>
+    <t>GoldDropMult</t>
+  </si>
+  <si>
+    <t>Multiplicateur de pièces d'or remportées après un combat</t>
+  </si>
+  <si>
+    <t>Encounter</t>
+  </si>
+  <si>
+    <t>MonsterId</t>
+  </si>
+  <si>
+    <t>SpawnChance</t>
+  </si>
+  <si>
+    <t>Identifiant de la rencontre</t>
+  </si>
+  <si>
+    <t>Clé importée de Square identifiant le monde où se situe la case à rencontre</t>
+  </si>
+  <si>
+    <t>Clé importée de Square identifiant la coordonnée X de la case à rencontre</t>
+  </si>
+  <si>
+    <t>Clé importée de Square identifiant la coordonnée Y de la case à rencontre</t>
+  </si>
+  <si>
+    <t>Clé importée de Monster identifiant le monstre provoquant la rencontre</t>
+  </si>
+  <si>
+    <t>Indicateur des chances de rencontres avec le/les monstre(s)</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t>TypeId</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Identifiant du monstre</t>
+  </si>
+  <si>
+    <t>Nom du monstre</t>
+  </si>
+  <si>
+    <t>Description du monstre</t>
+  </si>
+  <si>
+    <t>Clé importée de MonsterType identifiant le type du monstre</t>
+  </si>
+  <si>
+    <t>Niveau du monstre</t>
+  </si>
+  <si>
+    <t>Valeur de Force du monstre</t>
+  </si>
+  <si>
+    <t>Valeur de Dextérité du monstre</t>
+  </si>
+  <si>
+    <t>Valeur de Vitalité du monstre</t>
+  </si>
+  <si>
+    <t>Valeur d'Intelligence du monstre</t>
+  </si>
+  <si>
+    <t>Doit pointer sur un fichier existant</t>
+  </si>
+  <si>
+    <t>"Monster"</t>
+  </si>
+  <si>
+    <t>Nom du fichier image du monstre</t>
+  </si>
+  <si>
+    <t>dernier numéro de monstre utilisé + 1</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Identifiant de l'avatar du personnage</t>
+  </si>
+  <si>
+    <t>Nom du fichier image de l'avatar</t>
+  </si>
+  <si>
+    <t>Entier Long Non</t>
+  </si>
+  <si>
+    <t>dernier numéro d'avatar utilisé + 1</t>
+  </si>
+  <si>
+    <t>doit pointer un fichier existant</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Identifiant de la structure (village, dongeon, etc)</t>
+  </si>
+  <si>
+    <t>Clé importée de Square identifiant le monde où se trouve la structure</t>
+  </si>
+  <si>
+    <t>Clé importée de Square identifiant la position X de la structure</t>
+  </si>
+  <si>
+    <t>Clé importée de Square identifiant la position Y de la structure</t>
+  </si>
+  <si>
+    <t>Nom de la structure</t>
+  </si>
+  <si>
+    <t>Description de la structure</t>
+  </si>
+  <si>
+    <t>"A dark hole"</t>
+  </si>
+  <si>
+    <t>NonPlayerCharacter</t>
+  </si>
+  <si>
+    <t>Identifiant du personnage non-joueur (PNJ)</t>
+  </si>
+  <si>
+    <t>Clé importée de Square identifiant le monde du PNJ</t>
+  </si>
+  <si>
+    <t>Clé importée de Square indiquant la position X du PNJ sur la carte</t>
+  </si>
+  <si>
+    <t>Clé importée de Square indiquant la position Y du PNJ sur la carte</t>
+  </si>
+  <si>
+    <t>Nom du personnage non-joueur</t>
+  </si>
+  <si>
+    <t>Description du personnage non-joueur</t>
+  </si>
+  <si>
+    <t>"Lord Marc-Andre"</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="L24" sqref="L24:L25"/>
     </sheetView>
   </sheetViews>
@@ -2001,6 +2156,1299 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>255</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>255</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="38.85546875" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="8">
+        <v>40</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="L5" s="17"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="9">
+        <v>40</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="M13" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" customWidth="1"/>
+    <col min="13" max="13" width="3.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="9">
+        <v>40</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="M5" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>255</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>255</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="8">
+        <v>40</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="63" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="4.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>255</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>255</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="8">
+        <v>40</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2709,22 +4157,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="37.140625" customWidth="1"/>
+    <col min="12" max="12" width="38.42578125" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3205,54 +4653,87 @@
       <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="8">
+        <v>4</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>2</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9" t="s">
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="L19" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="M18" s="9"/>
+      <c r="M19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4624,10 +6105,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4636,7 +6117,7 @@
     <col min="2" max="2" width="66.140625" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" customWidth="1"/>
+    <col min="13" max="13" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4652,7 +6133,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4707,7 +6188,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -4721,7 +6202,9 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -4734,7 +6217,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E5" s="8">
         <v>0</v>
@@ -4748,7 +6231,9 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -4777,7 +6262,9 @@
       <c r="J6" s="8">
         <v>1</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
     </row>
@@ -4786,13 +6273,13 @@
         <v>226</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
@@ -4805,79 +6292,47 @@
       <c r="I7" s="8">
         <v>0</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="J7" s="8">
+        <v>10</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>10</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All tables created in dictionnary, but some updates still to do
</commit_message>
<xml_diff>
--- a/Fonctionnelle/Dictionnaire_Donnees.xlsx
+++ b/Fonctionnelle/Dictionnaire_Donnees.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="PlayerCharacter" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,16 @@
     <sheet name="Avatar" sheetId="13" r:id="rId12"/>
     <sheet name="Structure" sheetId="14" r:id="rId13"/>
     <sheet name="NonPlayerCharacter" sheetId="15" r:id="rId14"/>
+    <sheet name="GuildMember" sheetId="16" r:id="rId15"/>
+    <sheet name="Guild" sheetId="17" r:id="rId16"/>
+    <sheet name="GuildMessage" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="326">
   <si>
     <t>Nom du champ</t>
   </si>
@@ -888,6 +891,123 @@
   </si>
   <si>
     <t>"Lord Marc-Andre"</t>
+  </si>
+  <si>
+    <t>GuildMember</t>
+  </si>
+  <si>
+    <t>GuildId</t>
+  </si>
+  <si>
+    <t>PlayerRank</t>
+  </si>
+  <si>
+    <t>Clé importée de User identifiant le joueur membre de la guilde</t>
+  </si>
+  <si>
+    <t>Clé importée de Guild identifiant la guilde dont fait partie le joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicateur du rang du membre </t>
+  </si>
+  <si>
+    <t>Date de recrutement du joueur</t>
+  </si>
+  <si>
+    <t>GuildMemberRank*</t>
+  </si>
+  <si>
+    <t>GuildMemberRank</t>
+  </si>
+  <si>
+    <t>*Énumération pour les types de rangs: Propriétaire, Administrateur et Membre</t>
+  </si>
+  <si>
+    <t>Guild</t>
+  </si>
+  <si>
+    <t>Identifiant de la guilde</t>
+  </si>
+  <si>
+    <t>Nom de la guilde</t>
+  </si>
+  <si>
+    <t>Date de création de la guilde</t>
+  </si>
+  <si>
+    <t>Date de dernière connexion à la guilde</t>
+  </si>
+  <si>
+    <t>date du jour</t>
+  </si>
+  <si>
+    <t>Poster</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>GuildMessage</t>
+  </si>
+  <si>
+    <t>Identifiant du message de guilde</t>
+  </si>
+  <si>
+    <t>Clé importée de User identifiant le joueur ayant posté le message</t>
+  </si>
+  <si>
+    <t>Clé importée de Guild identifiant la guilde où est posté le message</t>
+  </si>
+  <si>
+    <t>Titre du message</t>
+  </si>
+  <si>
+    <t>Contenu du message</t>
+  </si>
+  <si>
+    <t>Date de création du message</t>
+  </si>
+  <si>
+    <t>Date de dernière modification du message</t>
+  </si>
+  <si>
+    <t>aaaa-mm-jj 00:00:00</t>
+  </si>
+  <si>
+    <t>ItemDropMult</t>
+  </si>
+  <si>
+    <t>Multiplicateur de l'objet pour les chances de gagner un objet après un combat</t>
+  </si>
+  <si>
+    <t>ItemDropMod</t>
+  </si>
+  <si>
+    <t>Valeur de modification de l'objet pour les chances de ramasser un objet après un combat</t>
+  </si>
+  <si>
+    <t>GoldDropMod</t>
+  </si>
+  <si>
+    <t>Valeur de modification de l'objet pour le gain d'or après un combat</t>
+  </si>
+  <si>
+    <t>-N</t>
+  </si>
+  <si>
+    <t>MinGold</t>
+  </si>
+  <si>
+    <t>MaxGold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur minimale de pièces d'or données lors d'une victoire du joueur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur maximale de pièces d'or données lors d'une victoire du joueur </t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1185,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1093,6 +1213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Commentaire" xfId="1" builtinId="10"/>
@@ -1401,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24:L25"/>
+    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,17 +2282,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:M3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="77.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
   </cols>
@@ -2399,37 +2520,99 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>4</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="9">
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8">
         <v>1</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3194,8 +3377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,18 +3635,669 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="43.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="83.85546875" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="8">
+        <v>40</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="4.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="8">
+        <v>40</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
@@ -3751,7 +4585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -4157,20 +4991,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="38.42578125" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
@@ -4654,10 +5488,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>236</v>
+        <v>315</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>237</v>
+        <v>316</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>18</v>
@@ -4686,54 +5520,87 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" s="8">
+        <v>4</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>2</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B20" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9" t="s">
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="L20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5239,19 +6106,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="63.7109375" customWidth="1"/>
+    <col min="2" max="2" width="83.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" customWidth="1"/>
     <col min="12" max="12" width="83.7109375" customWidth="1"/>
     <col min="13" max="13" width="4.28515625" customWidth="1"/>
@@ -5445,11 +6312,11 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J8" s="8">
-        <v>1000000</v>
+      <c r="I8" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K8" s="17">
         <v>0</v>
@@ -5478,11 +6345,11 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J9" s="8">
-        <v>1000000</v>
+      <c r="I9" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K9" s="17">
         <v>0</v>
@@ -5511,11 +6378,11 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J10" s="8">
-        <v>1000000</v>
+      <c r="I10" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K10" s="17">
         <v>0</v>
@@ -5544,11 +6411,11 @@
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J11" s="8">
-        <v>1000000</v>
+      <c r="I11" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K11" s="17">
         <v>0</v>
@@ -5577,11 +6444,11 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J12" s="8">
-        <v>1000000</v>
+      <c r="I12" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K12" s="17">
         <v>0</v>
@@ -5610,11 +6477,11 @@
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J13" s="8">
-        <v>1000000</v>
+      <c r="I13" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K13" s="17">
         <v>0</v>
@@ -5643,11 +6510,11 @@
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J14" s="8">
-        <v>1000000</v>
+      <c r="I14" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K14" s="17">
         <v>0</v>
@@ -5676,11 +6543,11 @@
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J15" s="8">
-        <v>1000000</v>
+      <c r="I15" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K15" s="17">
         <v>0</v>
@@ -5709,11 +6576,11 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J16" s="8">
-        <v>1000000</v>
+      <c r="I16" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K16" s="17">
         <v>0</v>
@@ -5723,10 +6590,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>18</v>
@@ -5742,33 +6609,33 @@
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="8">
-        <v>-1000000</v>
-      </c>
-      <c r="J17" s="8">
-        <v>1000000</v>
+      <c r="I17" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K17" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>193</v>
+        <v>317</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>208</v>
+        <v>318</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="E18" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>123</v>
@@ -5776,95 +6643,194 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8">
-        <v>-1000000</v>
+        <v>0</v>
       </c>
       <c r="J18" s="8">
-        <v>1000000</v>
+        <v>2</v>
       </c>
       <c r="K18" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+        <v>192</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="17"/>
+      <c r="I19" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0</v>
+      </c>
       <c r="L19" s="15"/>
       <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" s="8">
+        <v>4</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
+        <v>1</v>
+      </c>
+      <c r="K20" s="17">
+        <v>1</v>
+      </c>
+      <c r="L20" s="15"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="8">
+        <v>4</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8">
+        <v>2</v>
+      </c>
+      <c r="K21" s="17">
+        <v>1</v>
+      </c>
+      <c r="L21" s="15"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="17" t="s">
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L23" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="M20" s="8"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="9" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="18" t="s">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L24" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M24" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5876,8 +6842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:M3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6093,7 +7059,7 @@
       <c r="K8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="16" t="s">
         <v>74</v>
       </c>
       <c r="M8" s="9"/>
@@ -6107,8 +7073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:M3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6117,7 +7083,7 @@
     <col min="2" max="2" width="66.140625" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Maybe done with Data Dictionnary
</commit_message>
<xml_diff>
--- a/Fonctionnelle/Dictionnaire_Donnees.xlsx
+++ b/Fonctionnelle/Dictionnaire_Donnees.xlsx
@@ -4,33 +4,37 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="PlayerCharacter" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="2" r:id="rId2"/>
-    <sheet name="CharacterEquipement" sheetId="3" r:id="rId3"/>
-    <sheet name="ItemRoll" sheetId="4" r:id="rId4"/>
-    <sheet name="World" sheetId="5" r:id="rId5"/>
-    <sheet name="Square" sheetId="6" r:id="rId6"/>
-    <sheet name="Item" sheetId="7" r:id="rId7"/>
-    <sheet name="ItemCategory" sheetId="8" r:id="rId8"/>
-    <sheet name="EncounterDrop" sheetId="9" r:id="rId9"/>
-    <sheet name="Encounter" sheetId="11" r:id="rId10"/>
-    <sheet name="Monster" sheetId="12" r:id="rId11"/>
-    <sheet name="Avatar" sheetId="13" r:id="rId12"/>
-    <sheet name="Structure" sheetId="14" r:id="rId13"/>
-    <sheet name="NonPlayerCharacter" sheetId="15" r:id="rId14"/>
-    <sheet name="GuildMember" sheetId="16" r:id="rId15"/>
-    <sheet name="Guild" sheetId="17" r:id="rId16"/>
-    <sheet name="GuildMessage" sheetId="18" r:id="rId17"/>
+    <sheet name="Bank" sheetId="19" r:id="rId3"/>
+    <sheet name="CharacterEquipement" sheetId="3" r:id="rId4"/>
+    <sheet name="ItemRoll" sheetId="4" r:id="rId5"/>
+    <sheet name="World" sheetId="5" r:id="rId6"/>
+    <sheet name="Square" sheetId="6" r:id="rId7"/>
+    <sheet name="Item" sheetId="7" r:id="rId8"/>
+    <sheet name="ItemCategory" sheetId="8" r:id="rId9"/>
+    <sheet name="EncounterDrop" sheetId="9" r:id="rId10"/>
+    <sheet name="Encounter" sheetId="11" r:id="rId11"/>
+    <sheet name="Monster" sheetId="12" r:id="rId12"/>
+    <sheet name="Avatar" sheetId="13" r:id="rId13"/>
+    <sheet name="Structure" sheetId="14" r:id="rId14"/>
+    <sheet name="NonPlayerCharacter" sheetId="15" r:id="rId15"/>
+    <sheet name="GuildMember" sheetId="16" r:id="rId16"/>
+    <sheet name="Guild" sheetId="17" r:id="rId17"/>
+    <sheet name="GuildMessage" sheetId="18" r:id="rId18"/>
+    <sheet name="Shop" sheetId="20" r:id="rId19"/>
+    <sheet name="ShopSells" sheetId="21" r:id="rId20"/>
+    <sheet name="Skill" sheetId="22" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="364">
   <si>
     <t>Nom du champ</t>
   </si>
@@ -1008,6 +1012,120 @@
   </si>
   <si>
     <t xml:space="preserve">Valeur maximale de pièces d'or données lors d'une victoire du joueur </t>
+  </si>
+  <si>
+    <t>ShopId</t>
+  </si>
+  <si>
+    <t>Type de structure</t>
+  </si>
+  <si>
+    <t>Clé importée de Shop identifiant une boutique</t>
+  </si>
+  <si>
+    <t>StructureType</t>
+  </si>
+  <si>
+    <t>StructureType*</t>
+  </si>
+  <si>
+    <t>*enum {Camp, Village, City, Fort, Castle, Dungeon, MonsterCamp, Caravan, Bank}</t>
+  </si>
+  <si>
+    <t>BankId</t>
+  </si>
+  <si>
+    <t>Clé importée de Bank identifiant la banque du joueur</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>GoldAmount</t>
+  </si>
+  <si>
+    <t>Identifiant de la banque</t>
+  </si>
+  <si>
+    <t>Quantité de pièces d'or en banque</t>
+  </si>
+  <si>
+    <t>Date de dernière modification</t>
+  </si>
+  <si>
+    <t>Clé importée de Shop identifiant les achats reliés au PNJ</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>PriceMod</t>
+  </si>
+  <si>
+    <t>Identifiant de la boutique</t>
+  </si>
+  <si>
+    <t>Modificateur du prix des articles de la boutique</t>
+  </si>
+  <si>
+    <t>ShopSells</t>
+  </si>
+  <si>
+    <t>Sells</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Clé importée de Shop identifiant la boutique</t>
+  </si>
+  <si>
+    <t>Clé importée de ItemRoll identifiant l'objet vendu</t>
+  </si>
+  <si>
+    <t>Prix de vente de l'objet, sans modificateur</t>
+  </si>
+  <si>
+    <t>ManaCost</t>
+  </si>
+  <si>
+    <t>EnergyCost</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Identifiant du pouvoir</t>
+  </si>
+  <si>
+    <t>Nom du pouvoir</t>
+  </si>
+  <si>
+    <t>Description du pouvoir</t>
+  </si>
+  <si>
+    <t>Coût du pouvoir en points de Mana</t>
+  </si>
+  <si>
+    <t>Coût du pouvoir en points d'Énergie</t>
+  </si>
+  <si>
+    <t>Dégâts infligés par le pouvoir</t>
+  </si>
+  <si>
+    <t>Points de vie récupérés grâce au pouvoir</t>
+  </si>
+  <si>
+    <t>SkillId</t>
+  </si>
+  <si>
+    <t>Clé importée de Skill identifiant le pouvoir associé à l'objet</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1303,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1214,6 +1332,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Commentaire" xfId="1" builtinId="10"/>
@@ -1522,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,10 +2404,246 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>10</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>10</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,21 +2977,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:M3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
     <col min="12" max="12" width="38.85546875" customWidth="1"/>
     <col min="13" max="13" width="4.28515625" customWidth="1"/>
   </cols>
@@ -2747,7 +3106,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="17" t="s">
         <v>261</v>
       </c>
       <c r="L5" s="17"/>
@@ -2972,12 +3331,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:M3"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,18 +3470,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:M3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" customWidth="1"/>
+    <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" customWidth="1"/>
@@ -3346,39 +3706,103 @@
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="22">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" t="s">
+        <v>331</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:M3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3391,7 +3815,7 @@
     <col min="13" max="13" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -3399,7 +3823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -3407,7 +3831,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
@@ -3448,7 +3872,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -3481,7 +3905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
@@ -3514,7 +3938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -3547,7 +3971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -3580,7 +4004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
@@ -3607,35 +4031,65 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -3829,7 +4283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -4024,12 +4478,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4039,7 +4493,7 @@
     <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4285,18 +4739,160 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="9">
+        <v>4</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>4</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
@@ -4491,39 +5087,33 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>44</v>
+        <v>332</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>92</v>
+        <v>333</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>73</v>
-      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="8" t="s">
-        <v>74</v>
-      </c>
+      <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>46</v>
@@ -4543,34 +5133,63 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="8"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4581,7 +5200,629 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="8">
+        <v>40</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8">
+        <v>3</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="8">
+        <v>3</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="23">
+        <v>0</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E11" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
@@ -4989,7 +6230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
@@ -5607,7 +6848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -5865,7 +7106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -6104,12 +7345,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6772,65 +8013,94 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>44</v>
+        <v>362</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>151</v>
+        <v>363</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
       <c r="F23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>73</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="17" t="s">
+      <c r="K23" s="17"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="L23" s="15" t="s">
+      <c r="L24" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="M23" s="8"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B25" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="9" t="s">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="18" t="s">
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="L24" s="16" t="s">
+      <c r="L25" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="M24" s="9"/>
+      <c r="M25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6838,7 +8108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
@@ -7067,240 +8337,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="8">
-        <v>4</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>10</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>10</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added AnalyseOrg. It has begun
</commit_message>
<xml_diff>
--- a/Fonctionnelle/Dictionnaire_Donnees.xlsx
+++ b/Fonctionnelle/Dictionnaire_Donnees.xlsx
@@ -1203,9 +1203,6 @@
     <t>Mana Max</t>
   </si>
   <si>
-    <t>Mana Max = Intellect * 5</t>
-  </si>
-  <si>
     <t>IsDead = true si CurrentHealth &lt;= 0</t>
   </si>
   <si>
@@ -1588,6 +1585,10 @@
   <si>
     <t>Générée par le système; modifiable uniquement 
 par le système de manière transparente; &lt;= date du jour</t>
+  </si>
+  <si>
+    <t>Mana Max = (Intellect * 5) * 
+(ItemRoll.ManaMult * Item.ManaMod)</t>
   </si>
 </sst>
 </file>
@@ -2282,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -2824,11 +2825,11 @@
         <v>374</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -2858,8 +2859,8 @@
       <c r="K17" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>377</v>
+      <c r="L17" s="15" t="s">
+        <v>490</v>
       </c>
       <c r="M17" s="17"/>
     </row>
@@ -2987,7 +2988,7 @@
         <v>299</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M21" s="17"/>
     </row>
@@ -3043,7 +3044,7 @@
         <v>44</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M23" s="17"/>
     </row>
@@ -3074,7 +3075,7 @@
         <v>44</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M24" s="24"/>
     </row>
@@ -3238,7 +3239,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M31" s="5"/>
     </row>
@@ -3263,7 +3264,7 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M32" s="5"/>
     </row>
@@ -3317,7 +3318,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M34" s="5"/>
     </row>
@@ -3346,7 +3347,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M35" s="5"/>
     </row>
@@ -3545,7 +3546,7 @@
         <v>44</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="M43" s="6"/>
     </row>
@@ -3628,7 +3629,7 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M47" s="5" t="s">
         <v>95</v>
@@ -3655,7 +3656,7 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
       <c r="L48" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M48" s="5" t="s">
         <v>22</v>
@@ -3682,7 +3683,7 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>22</v>
@@ -3709,7 +3710,7 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>22</v>
@@ -3736,7 +3737,7 @@
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
       <c r="L51" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>22</v>
@@ -3763,7 +3764,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M52" s="5" t="s">
         <v>22</v>
@@ -3790,7 +3791,7 @@
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
       <c r="L53" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>22</v>
@@ -3817,7 +3818,7 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>22</v>
@@ -3844,7 +3845,7 @@
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>22</v>
@@ -3871,7 +3872,7 @@
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>22</v>
@@ -3898,7 +3899,7 @@
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M57" s="5" t="s">
         <v>22</v>
@@ -3925,7 +3926,7 @@
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
       <c r="L58" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M58" s="6" t="s">
         <v>22</v>
@@ -4082,7 +4083,7 @@
         <v>1</v>
       </c>
       <c r="L64" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M64" s="5"/>
     </row>
@@ -4117,7 +4118,7 @@
         <v>1</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M65" s="5"/>
     </row>
@@ -4152,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M66" s="5"/>
     </row>
@@ -4187,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M67" s="5"/>
     </row>
@@ -4222,7 +4223,7 @@
         <v>1</v>
       </c>
       <c r="L68" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M68" s="5"/>
     </row>
@@ -4257,7 +4258,7 @@
         <v>1</v>
       </c>
       <c r="L69" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M69" s="5"/>
     </row>
@@ -4292,7 +4293,7 @@
         <v>1</v>
       </c>
       <c r="L70" s="15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M70" s="5"/>
     </row>
@@ -4327,7 +4328,7 @@
         <v>1</v>
       </c>
       <c r="L71" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M71" s="5"/>
     </row>
@@ -4362,7 +4363,7 @@
         <v>1</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M72" s="5"/>
     </row>
@@ -4397,7 +4398,7 @@
         <v>1</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M73" s="5"/>
     </row>
@@ -4432,7 +4433,7 @@
         <v>1</v>
       </c>
       <c r="L74" s="15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="M74" s="5"/>
     </row>
@@ -4467,7 +4468,7 @@
         <v>1</v>
       </c>
       <c r="L75" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M75" s="5"/>
     </row>
@@ -4502,7 +4503,7 @@
         <v>1</v>
       </c>
       <c r="L76" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M76" s="5"/>
     </row>
@@ -4673,10 +4674,10 @@
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
       <c r="K83" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="L83" s="5" t="s">
         <v>409</v>
-      </c>
-      <c r="L83" s="5" t="s">
-        <v>410</v>
       </c>
       <c r="M83" s="5"/>
     </row>
@@ -4764,15 +4765,15 @@
         <v>17</v>
       </c>
       <c r="G86" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="H86" s="5" t="s">
         <v>412</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>413</v>
       </c>
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
       <c r="K86" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L86" s="5"/>
       <c r="M86" s="5"/>
@@ -4800,7 +4801,7 @@
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
       <c r="L87" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M87" s="6"/>
     </row>
@@ -4926,7 +4927,7 @@
       </c>
       <c r="K92" s="5"/>
       <c r="L92" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M92" s="5" t="s">
         <v>19</v>
@@ -4961,7 +4962,7 @@
       </c>
       <c r="K93" s="5"/>
       <c r="L93" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M93" s="5" t="s">
         <v>19</v>
@@ -4990,7 +4991,7 @@
       <c r="J94" s="6"/>
       <c r="K94" s="6"/>
       <c r="L94" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M94" s="6"/>
     </row>
@@ -5105,10 +5106,10 @@
       <c r="I99" s="43"/>
       <c r="J99" s="43"/>
       <c r="K99" s="43" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L99" s="43" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M99" s="43"/>
     </row>
@@ -5135,7 +5136,7 @@
         <v>363</v>
       </c>
       <c r="L100" s="43" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M100" s="43"/>
     </row>
@@ -5205,7 +5206,7 @@
         <v>0</v>
       </c>
       <c r="L102" s="43" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M102" s="43"/>
     </row>
@@ -5240,7 +5241,7 @@
         <v>0</v>
       </c>
       <c r="L103" s="43" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M103" s="43"/>
     </row>
@@ -5275,7 +5276,7 @@
         <v>0</v>
       </c>
       <c r="L104" s="43" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M104" s="43"/>
     </row>
@@ -5310,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="L105" s="43" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M105" s="43"/>
     </row>
@@ -5345,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="L106" s="46" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M106" s="43"/>
     </row>
@@ -5380,7 +5381,7 @@
         <v>0</v>
       </c>
       <c r="L107" s="46" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M107" s="43"/>
     </row>
@@ -5415,7 +5416,7 @@
         <v>0</v>
       </c>
       <c r="L108" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="M108" s="43"/>
     </row>
@@ -5450,7 +5451,7 @@
         <v>0</v>
       </c>
       <c r="L109" s="46" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M109" s="43"/>
     </row>
@@ -5485,7 +5486,7 @@
         <v>0</v>
       </c>
       <c r="L110" s="46" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M110" s="43"/>
     </row>
@@ -5520,7 +5521,7 @@
         <v>1</v>
       </c>
       <c r="L111" s="46" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="M111" s="43"/>
     </row>
@@ -5555,7 +5556,7 @@
         <v>1</v>
       </c>
       <c r="L112" s="43" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M112" s="43"/>
     </row>
@@ -5590,7 +5591,7 @@
         <v>0</v>
       </c>
       <c r="L113" s="43" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M113" s="43"/>
     </row>
@@ -5625,7 +5626,7 @@
         <v>1</v>
       </c>
       <c r="L114" s="43" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M114" s="43"/>
     </row>
@@ -5660,16 +5661,16 @@
         <v>1</v>
       </c>
       <c r="L115" s="43" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M115" s="43"/>
     </row>
     <row r="116" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="42" t="s">
+        <v>469</v>
+      </c>
+      <c r="B116" s="44" t="s">
         <v>470</v>
-      </c>
-      <c r="B116" s="44" t="s">
-        <v>471</v>
       </c>
       <c r="C116" s="42" t="s">
         <v>15</v>
@@ -5743,7 +5744,7 @@
       <c r="J118" s="43"/>
       <c r="K118" s="43"/>
       <c r="L118" s="43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M118" s="43" t="s">
         <v>22</v>
@@ -5776,7 +5777,7 @@
         <v>171</v>
       </c>
       <c r="L119" s="46" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M119" s="43"/>
     </row>
@@ -5807,7 +5808,7 @@
         <v>171</v>
       </c>
       <c r="L120" s="46" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M120" s="43"/>
     </row>
@@ -5842,7 +5843,7 @@
         <v>1</v>
       </c>
       <c r="L121" s="53" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="M121" s="51"/>
     </row>
@@ -6011,10 +6012,10 @@
       <c r="I127" s="5"/>
       <c r="J127" s="5"/>
       <c r="K127" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="L127" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M127" s="5"/>
     </row>
@@ -6041,7 +6042,7 @@
         <v>363</v>
       </c>
       <c r="L128" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M128" s="5"/>
     </row>
@@ -6139,7 +6140,7 @@
         <v>102</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>15</v>
@@ -6159,7 +6160,7 @@
       <c r="J133" s="5"/>
       <c r="K133" s="5"/>
       <c r="L133" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M133" s="5" t="s">
         <v>95</v>
@@ -6170,7 +6171,7 @@
         <v>183</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>15</v>
@@ -6190,7 +6191,7 @@
       <c r="J134" s="5"/>
       <c r="K134" s="5"/>
       <c r="L134" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M134" s="5" t="s">
         <v>95</v>
@@ -6260,7 +6261,7 @@
         <v>0</v>
       </c>
       <c r="L136" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M136" s="5"/>
     </row>
@@ -6295,7 +6296,7 @@
         <v>0</v>
       </c>
       <c r="L137" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M137" s="6"/>
     </row>
@@ -6386,7 +6387,7 @@
       </c>
       <c r="K141" s="5"/>
       <c r="L141" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M141" s="5" t="s">
         <v>19</v>
@@ -6421,7 +6422,7 @@
       </c>
       <c r="K142" s="5"/>
       <c r="L142" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M142" s="5" t="s">
         <v>22</v>
@@ -6456,7 +6457,7 @@
       </c>
       <c r="K143" s="5"/>
       <c r="L143" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="M143" s="5" t="s">
         <v>22</v>
@@ -6491,7 +6492,7 @@
       </c>
       <c r="K144" s="5"/>
       <c r="L144" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="M144" s="5" t="s">
         <v>22</v>
@@ -6526,7 +6527,7 @@
       </c>
       <c r="K145" s="5"/>
       <c r="L145" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="M145" s="5" t="s">
         <v>22</v>
@@ -6594,7 +6595,7 @@
       </c>
       <c r="K147" s="5"/>
       <c r="L147" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="M147" s="5"/>
     </row>
@@ -6627,7 +6628,7 @@
       </c>
       <c r="K148" s="6"/>
       <c r="L148" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="M148" s="6"/>
     </row>
@@ -6745,7 +6746,7 @@
         <v>214</v>
       </c>
       <c r="L153" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M153" s="5"/>
     </row>
@@ -6772,7 +6773,7 @@
         <v>363</v>
       </c>
       <c r="L154" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M154" s="5"/>
     </row>
@@ -6805,7 +6806,7 @@
       </c>
       <c r="K155" s="5"/>
       <c r="L155" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M155" s="5" t="s">
         <v>22</v>
@@ -6999,7 +7000,7 @@
       <c r="J161" s="6"/>
       <c r="K161" s="6"/>
       <c r="L161" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M161" s="6"/>
     </row>
@@ -7119,7 +7120,7 @@
       <c r="J166" s="6"/>
       <c r="K166" s="6"/>
       <c r="L166" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="M166" s="6"/>
     </row>
@@ -7210,7 +7211,7 @@
       </c>
       <c r="K170" s="5"/>
       <c r="L170" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M170" s="5" t="s">
         <v>19</v>
@@ -7245,7 +7246,7 @@
       </c>
       <c r="K171" s="5"/>
       <c r="L171" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="M171" s="5" t="s">
         <v>22</v>
@@ -7280,7 +7281,7 @@
       </c>
       <c r="K172" s="5"/>
       <c r="L172" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="M172" s="5" t="s">
         <v>22</v>
@@ -7315,7 +7316,7 @@
       </c>
       <c r="K173" s="5"/>
       <c r="L173" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="M173" s="5" t="s">
         <v>22</v>
@@ -7346,7 +7347,7 @@
         <v>227</v>
       </c>
       <c r="L174" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M174" s="5"/>
     </row>
@@ -7371,7 +7372,7 @@
       <c r="J175" s="5"/>
       <c r="K175" s="5"/>
       <c r="L175" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M175" s="5"/>
     </row>
@@ -7396,7 +7397,7 @@
       <c r="J176" s="5"/>
       <c r="K176" s="5"/>
       <c r="L176" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M176" s="5"/>
     </row>
@@ -7429,7 +7430,7 @@
       </c>
       <c r="K177" s="6"/>
       <c r="L177" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="M177" s="6" t="s">
         <v>22</v>
@@ -7530,7 +7531,7 @@
       </c>
       <c r="K182" s="5"/>
       <c r="L182" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M182" s="5" t="s">
         <v>19</v>
@@ -7565,7 +7566,7 @@
       </c>
       <c r="K183" s="5"/>
       <c r="L183" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M183" s="5" t="s">
         <v>22</v>
@@ -7600,7 +7601,7 @@
       </c>
       <c r="K184" s="5"/>
       <c r="L184" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="M184" s="5" t="s">
         <v>22</v>
@@ -7635,7 +7636,7 @@
       </c>
       <c r="K185" s="5"/>
       <c r="L185" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="M185" s="5" t="s">
         <v>22</v>
@@ -7666,7 +7667,7 @@
         <v>232</v>
       </c>
       <c r="L186" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M186" s="5"/>
     </row>
@@ -7693,7 +7694,7 @@
         <v>363</v>
       </c>
       <c r="L187" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M187" s="5"/>
     </row>
@@ -7722,7 +7723,7 @@
       <c r="J188" s="26"/>
       <c r="K188" s="26"/>
       <c r="L188" s="54" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="M188" s="26" t="s">
         <v>22</v>
@@ -7861,7 +7862,7 @@
       <c r="J194" s="5"/>
       <c r="K194" s="5"/>
       <c r="L194" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="M194" s="5"/>
     </row>
@@ -7890,7 +7891,7 @@
       <c r="J195" s="6"/>
       <c r="K195" s="6"/>
       <c r="L195" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M195" s="6"/>
     </row>
@@ -8011,10 +8012,10 @@
       <c r="I201" s="5"/>
       <c r="J201" s="5"/>
       <c r="K201" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L201" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="M201" s="5"/>
     </row>
@@ -8045,7 +8046,7 @@
         <v>44</v>
       </c>
       <c r="L202" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M202" s="5"/>
     </row>
@@ -8076,7 +8077,7 @@
         <v>44</v>
       </c>
       <c r="L203" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M203" s="6"/>
     </row>
@@ -8241,10 +8242,10 @@
       <c r="I210" s="5"/>
       <c r="J210" s="5"/>
       <c r="K210" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L210" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M210" s="5"/>
     </row>
@@ -8271,7 +8272,7 @@
         <v>363</v>
       </c>
       <c r="L211" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M211" s="5"/>
     </row>
@@ -8302,7 +8303,7 @@
         <v>44</v>
       </c>
       <c r="L212" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M212" s="5"/>
     </row>
@@ -8333,7 +8334,7 @@
         <v>44</v>
       </c>
       <c r="L213" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M213" s="6"/>
     </row>
@@ -8420,7 +8421,7 @@
       <c r="J217" s="5"/>
       <c r="K217" s="5"/>
       <c r="L217" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="M217" s="5" t="s">
         <v>19</v>
@@ -8542,7 +8543,7 @@
       <c r="J222" s="5"/>
       <c r="K222" s="5"/>
       <c r="L222" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="M222" s="5" t="s">
         <v>95</v>
@@ -8695,7 +8696,7 @@
       </c>
       <c r="K228" s="5"/>
       <c r="L228" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M228" s="5" t="s">
         <v>19</v>
@@ -8724,7 +8725,7 @@
       <c r="J229" s="5"/>
       <c r="K229" s="5"/>
       <c r="L229" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M229" s="5"/>
     </row>
@@ -8749,7 +8750,7 @@
       <c r="J230" s="5"/>
       <c r="K230" s="5"/>
       <c r="L230" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M230" s="5"/>
     </row>
@@ -9078,7 +9079,7 @@
         <v>44</v>
       </c>
       <c r="L242" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M242" s="5"/>
     </row>
@@ -9107,7 +9108,7 @@
         <v>364</v>
       </c>
       <c r="L243" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M243" s="5"/>
     </row>
@@ -9134,7 +9135,7 @@
         <v>363</v>
       </c>
       <c r="L244" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M244" s="6"/>
     </row>
@@ -9144,7 +9145,7 @@
       <c r="C246" s="12"/>
       <c r="D246" s="28"/>
       <c r="E246" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F246" s="28"/>
       <c r="G246" s="12"/>
@@ -9201,7 +9202,7 @@
         <v>13</v>
       </c>
       <c r="B248" s="32" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C248" s="32" t="s">
         <v>15</v>
@@ -9225,7 +9226,7 @@
       </c>
       <c r="K248" s="55"/>
       <c r="L248" s="55" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M248" s="5" t="s">
         <v>19</v>
@@ -9236,7 +9237,7 @@
         <v>23</v>
       </c>
       <c r="B249" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C249" s="32" t="s">
         <v>60</v>
@@ -9253,10 +9254,10 @@
       <c r="I249" s="55"/>
       <c r="J249" s="55"/>
       <c r="K249" s="55" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L249" s="55" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M249" s="5"/>
     </row>
@@ -9265,7 +9266,7 @@
         <v>1</v>
       </c>
       <c r="B250" s="33" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C250" s="33" t="s">
         <v>80</v>
@@ -9283,7 +9284,7 @@
         <v>363</v>
       </c>
       <c r="L250" s="56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M250" s="6"/>
     </row>
@@ -9293,7 +9294,7 @@
       <c r="C252" s="12"/>
       <c r="D252" s="28"/>
       <c r="E252" s="13" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F252" s="28"/>
       <c r="G252" s="12"/>
@@ -9350,7 +9351,7 @@
         <v>13</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>70</v>
@@ -9374,10 +9375,10 @@
     </row>
     <row r="255" spans="1:13" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B255" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>70</v>
@@ -9393,7 +9394,7 @@
       <c r="J255" s="5"/>
       <c r="K255" s="5"/>
       <c r="L255" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M255" s="5" t="s">
         <v>22</v>
@@ -9404,7 +9405,7 @@
         <v>20</v>
       </c>
       <c r="B256" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>70</v>
@@ -9420,7 +9421,7 @@
       <c r="J256" s="5"/>
       <c r="K256" s="5"/>
       <c r="L256" s="15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M256" s="5" t="s">
         <v>22</v>
@@ -9428,10 +9429,10 @@
     </row>
     <row r="257" spans="1:13" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B257" s="20" t="s">
         <v>473</v>
-      </c>
-      <c r="B257" s="20" t="s">
-        <v>474</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>15</v>
@@ -9457,7 +9458,7 @@
         <v>1</v>
       </c>
       <c r="L257" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M257" s="6"/>
     </row>
@@ -9467,7 +9468,7 @@
       <c r="C259" s="12"/>
       <c r="D259" s="28"/>
       <c r="E259" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F259" s="28"/>
       <c r="G259" s="12"/>
@@ -9524,7 +9525,7 @@
         <v>13</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>70</v>
@@ -9548,10 +9549,10 @@
     </row>
     <row r="262" spans="1:13" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>70</v>
@@ -9567,7 +9568,7 @@
       <c r="J262" s="4"/>
       <c r="K262" s="5"/>
       <c r="L262" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M262" s="5" t="s">
         <v>22</v>
@@ -9575,10 +9576,10 @@
     </row>
     <row r="263" spans="1:13" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B263" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>70</v>
@@ -9594,7 +9595,7 @@
       <c r="J263" s="4"/>
       <c r="K263" s="5"/>
       <c r="L263" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="M263" s="5" t="s">
         <v>22</v>
@@ -9605,7 +9606,7 @@
         <v>41</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C264" s="2" t="s">
         <v>43</v>
@@ -9627,7 +9628,7 @@
         <v>44</v>
       </c>
       <c r="L264" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M264" s="6"/>
     </row>

</xml_diff>